<commit_message>
wrote first var / mean code for innings
</commit_message>
<xml_diff>
--- a/Known python issues.xlsx
+++ b/Known python issues.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MSc\Thesis\Breaking the Higher Load\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88E25623-5F85-4C30-B324-B7F52F6A6976}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A337D0A-80CE-4336-991F-697BB104ACF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{ED9FAEDA-F60E-42FC-910F-5E369763F547}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{ED9FAEDA-F60E-42FC-910F-5E369763F547}"/>
   </bookViews>
   <sheets>
     <sheet name="Bugs and errors" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="43">
   <si>
     <t>found by</t>
   </si>
@@ -159,6 +159,12 @@
   </si>
   <si>
     <t>Thomas_workspace</t>
+  </si>
+  <si>
+    <t>Added missing data catches in mains</t>
+  </si>
+  <si>
+    <t>Var / mean of inning</t>
   </si>
 </sst>
 </file>
@@ -194,9 +200,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -514,7 +521,7 @@
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -854,16 +861,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6043AC44-27D4-44BA-A4A5-A7B72C27DCEA}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="40.140625" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" style="2" customWidth="1"/>
     <col min="4" max="4" width="10.5703125" customWidth="1"/>
     <col min="5" max="5" width="12.85546875" customWidth="1"/>
     <col min="6" max="6" width="18.140625" customWidth="1"/>
@@ -873,7 +880,7 @@
       <c r="A1" t="s">
         <v>29</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>31</v>
       </c>
       <c r="C1" t="s">
@@ -896,7 +903,7 @@
       <c r="A2" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="2">
         <v>44645</v>
       </c>
       <c r="C2" t="s">
@@ -907,7 +914,7 @@
       <c r="A3" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="2">
         <v>44645</v>
       </c>
       <c r="C3" t="s">
@@ -918,7 +925,7 @@
       <c r="A4" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="2">
         <v>44645</v>
       </c>
       <c r="C4" t="s">
@@ -929,16 +936,38 @@
       <c r="A5" t="s">
         <v>39</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="2">
         <v>44645</v>
       </c>
       <c r="C5" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="1">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="2">
         <v>44645</v>
       </c>
-      <c r="F5" t="s">
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="2">
+        <v>44645</v>
+      </c>
+      <c r="C7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="1">
+        <v>44645</v>
+      </c>
+      <c r="F7" t="s">
         <v>40</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Change to calc_omega, and added some visualization of sEMG
</commit_message>
<xml_diff>
--- a/Known python issues.xlsx
+++ b/Known python issues.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MSc\Thesis\Breaking the Higher Load\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A337D0A-80CE-4336-991F-697BB104ACF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71335AEB-7723-4637-9D46-BFE1759C128B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{ED9FAEDA-F60E-42FC-910F-5E369763F547}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{ED9FAEDA-F60E-42FC-910F-5E369763F547}"/>
   </bookViews>
   <sheets>
     <sheet name="Bugs and errors" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="48">
   <si>
     <t>found by</t>
   </si>
@@ -165,6 +165,21 @@
   </si>
   <si>
     <t>Var / mean of inning</t>
+  </si>
+  <si>
+    <t>Ton</t>
+  </si>
+  <si>
+    <t>f.calc_omega uses 3x1 vectors</t>
+  </si>
+  <si>
+    <t>fixed vector notation and associated matrix math</t>
+  </si>
+  <si>
+    <t>Faulty pitch remover in main_template</t>
+  </si>
+  <si>
+    <t>Rotation of new optitrack dataset</t>
   </si>
 </sst>
 </file>
@@ -521,7 +536,7 @@
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -767,9 +782,7 @@
       <c r="C9" t="s">
         <v>2</v>
       </c>
-      <c r="I9" s="1" t="s">
-        <v>19</v>
-      </c>
+      <c r="I9" s="1"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -801,7 +814,27 @@
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="I11" s="1"/>
+      <c r="B11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" s="1">
+        <v>44649</v>
+      </c>
+      <c r="E11" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" t="s">
+        <v>45</v>
+      </c>
+      <c r="G11" s="1">
+        <v>44649</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -861,18 +894,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6043AC44-27D4-44BA-A4A5-A7B72C27DCEA}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="40.140625" customWidth="1"/>
     <col min="2" max="2" width="11.85546875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" customWidth="1"/>
     <col min="6" max="6" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -909,6 +942,12 @@
       <c r="C2" t="s">
         <v>2</v>
       </c>
+      <c r="E2" s="1">
+        <v>44645</v>
+      </c>
+      <c r="F2" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -920,6 +959,12 @@
       <c r="C3" t="s">
         <v>2</v>
       </c>
+      <c r="E3" s="1">
+        <v>44645</v>
+      </c>
+      <c r="F3" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -931,6 +976,12 @@
       <c r="C4" t="s">
         <v>2</v>
       </c>
+      <c r="E4" s="1">
+        <v>44645</v>
+      </c>
+      <c r="F4" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -942,6 +993,12 @@
       <c r="C5" t="s">
         <v>2</v>
       </c>
+      <c r="E5" s="1">
+        <v>44645</v>
+      </c>
+      <c r="F5" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -953,6 +1010,12 @@
       <c r="C6" t="s">
         <v>2</v>
       </c>
+      <c r="E6" s="1">
+        <v>44645</v>
+      </c>
+      <c r="F6" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -968,6 +1031,40 @@
         <v>44645</v>
       </c>
       <c r="F7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="2">
+        <v>44648</v>
+      </c>
+      <c r="C8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="1">
+        <v>44648</v>
+      </c>
+      <c r="F8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" s="2">
+        <v>44643</v>
+      </c>
+      <c r="C9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="1">
+        <v>44643</v>
+      </c>
+      <c r="F9" t="s">
         <v>40</v>
       </c>
     </row>

</xml_diff>

<commit_message>
pretty mean + var plot
</commit_message>
<xml_diff>
--- a/Known python issues.xlsx
+++ b/Known python issues.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MSc\Thesis\Breaking the Higher Load\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71335AEB-7723-4637-9D46-BFE1759C128B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6654FC85-21B7-4AEC-8AE9-B945EFA0803C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{ED9FAEDA-F60E-42FC-910F-5E369763F547}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{ED9FAEDA-F60E-42FC-910F-5E369763F547}"/>
   </bookViews>
   <sheets>
     <sheet name="Bugs and errors" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="49">
   <si>
     <t>found by</t>
   </si>
@@ -155,18 +155,12 @@
     <t>f.time_sync functions added</t>
   </si>
   <si>
-    <t>Added python tracking file</t>
-  </si>
-  <si>
     <t>Thomas_workspace</t>
   </si>
   <si>
     <t>Added missing data catches in mains</t>
   </si>
   <si>
-    <t>Var / mean of inning</t>
-  </si>
-  <si>
     <t>Ton</t>
   </si>
   <si>
@@ -179,7 +173,16 @@
     <t>Faulty pitch remover in main_template</t>
   </si>
   <si>
-    <t>Rotation of new optitrack dataset</t>
+    <t>Added python changelog excel file</t>
+  </si>
+  <si>
+    <t>f.calc_variability_seg_M_joint</t>
+  </si>
+  <si>
+    <t>f.orient_markers</t>
+  </si>
+  <si>
+    <t>Orients markers to match old data set</t>
   </si>
 </sst>
 </file>
@@ -535,8 +538,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77D5D533-2F00-419B-A737-80ACEFF3460C}">
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -815,19 +818,19 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C11" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D11" s="1">
         <v>44649</v>
       </c>
       <c r="E11" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" t="s">
         <v>43</v>
-      </c>
-      <c r="F11" t="s">
-        <v>45</v>
       </c>
       <c r="G11" s="1">
         <v>44649</v>
@@ -896,15 +899,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6043AC44-27D4-44BA-A4A5-A7B72C27DCEA}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="40.140625" customWidth="1"/>
     <col min="2" max="2" width="11.85546875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" customWidth="1"/>
+    <col min="4" max="4" width="43.42578125" customWidth="1"/>
     <col min="5" max="5" width="18.7109375" customWidth="1"/>
     <col min="6" max="6" width="18.140625" customWidth="1"/>
   </cols>
@@ -946,7 +949,7 @@
         <v>44645</v>
       </c>
       <c r="F2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -963,7 +966,7 @@
         <v>44645</v>
       </c>
       <c r="F3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -980,29 +983,29 @@
         <v>44645</v>
       </c>
       <c r="F4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" s="2">
+        <v>44645</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="1">
+        <v>44645</v>
+      </c>
+      <c r="F5" t="s">
         <v>39</v>
-      </c>
-      <c r="B5" s="2">
-        <v>44645</v>
-      </c>
-      <c r="C5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E5" s="1">
-        <v>44645</v>
-      </c>
-      <c r="F5" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B6" s="2">
         <v>44645</v>
@@ -1014,12 +1017,12 @@
         <v>44645</v>
       </c>
       <c r="F6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B7" s="2">
         <v>44645</v>
@@ -1031,12 +1034,12 @@
         <v>44645</v>
       </c>
       <c r="F7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B8" s="2">
         <v>44648</v>
@@ -1048,7 +1051,7 @@
         <v>44648</v>
       </c>
       <c r="F8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1061,11 +1064,14 @@
       <c r="C9" t="s">
         <v>2</v>
       </c>
+      <c r="D9" t="s">
+        <v>48</v>
+      </c>
       <c r="E9" s="1">
         <v>44643</v>
       </c>
       <c r="F9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
temp changes, remote work
</commit_message>
<xml_diff>
--- a/Known python issues.xlsx
+++ b/Known python issues.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MSc\Thesis\Breaking the Higher Load\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6654FC85-21B7-4AEC-8AE9-B945EFA0803C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D11BBD49-069E-4149-9B0E-EC628A11B54D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{ED9FAEDA-F60E-42FC-910F-5E369763F547}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{ED9FAEDA-F60E-42FC-910F-5E369763F547}"/>
   </bookViews>
   <sheets>
     <sheet name="Bugs and errors" sheetId="1" r:id="rId1"/>
-    <sheet name="Implemented Features" sheetId="2" r:id="rId2"/>
+    <sheet name="Features  To dos" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="51">
   <si>
     <t>found by</t>
   </si>
@@ -137,9 +137,6 @@
     <t>Commited on</t>
   </si>
   <si>
-    <t>Comments</t>
-  </si>
-  <si>
     <t>f.plot_inning_segment_moments</t>
   </si>
   <si>
@@ -183,6 +180,15 @@
   </si>
   <si>
     <t>Orients markers to match old data set</t>
+  </si>
+  <si>
+    <t>mean / var if data set sufficent</t>
+  </si>
+  <si>
+    <t>Changes</t>
+  </si>
+  <si>
+    <t>main</t>
   </si>
 </sst>
 </file>
@@ -538,7 +544,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77D5D533-2F00-419B-A737-80ACEFF3460C}">
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
@@ -766,7 +772,7 @@
         <v>2</v>
       </c>
       <c r="F8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G8" s="1">
         <v>44645</v>
@@ -804,7 +810,7 @@
         <v>2</v>
       </c>
       <c r="F10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G10" s="1">
         <v>44645</v>
@@ -818,19 +824,19 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D11" s="1">
         <v>44649</v>
       </c>
       <c r="E11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G11" s="1">
         <v>44649</v>
@@ -897,17 +903,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6043AC44-27D4-44BA-A4A5-A7B72C27DCEA}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="40.140625" customWidth="1"/>
     <col min="2" max="2" width="11.85546875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="43.42578125" customWidth="1"/>
+    <col min="4" max="4" width="51.7109375" customWidth="1"/>
     <col min="5" max="5" width="18.7109375" customWidth="1"/>
     <col min="6" max="6" width="18.140625" customWidth="1"/>
   </cols>
@@ -923,7 +929,7 @@
         <v>30</v>
       </c>
       <c r="D1" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="E1" t="s">
         <v>32</v>
@@ -937,7 +943,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B2" s="2">
         <v>44645</v>
@@ -949,12 +955,12 @@
         <v>44645</v>
       </c>
       <c r="F2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B3" s="2">
         <v>44645</v>
@@ -966,12 +972,12 @@
         <v>44645</v>
       </c>
       <c r="F3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B4" s="2">
         <v>44645</v>
@@ -983,12 +989,12 @@
         <v>44645</v>
       </c>
       <c r="F4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B5" s="2">
         <v>44645</v>
@@ -1000,12 +1006,12 @@
         <v>44645</v>
       </c>
       <c r="F5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B6" s="2">
         <v>44645</v>
@@ -1017,12 +1023,12 @@
         <v>44645</v>
       </c>
       <c r="F6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B7" s="2">
         <v>44645</v>
@@ -1034,12 +1040,12 @@
         <v>44645</v>
       </c>
       <c r="F7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B8" s="2">
         <v>44648</v>
@@ -1051,12 +1057,12 @@
         <v>44648</v>
       </c>
       <c r="F8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B9" s="2">
         <v>44643</v>
@@ -1065,13 +1071,33 @@
         <v>2</v>
       </c>
       <c r="D9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E9" s="1">
         <v>44643</v>
       </c>
       <c r="F9" t="s">
-        <v>39</v>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" s="2">
+        <v>44643</v>
+      </c>
+      <c r="C10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" s="1">
+        <v>44643</v>
+      </c>
+      <c r="F10" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added new way to track output data, and auto run whole innings
</commit_message>
<xml_diff>
--- a/Known python issues.xlsx
+++ b/Known python issues.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MSc\Thesis\Breaking the Higher Load\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D11BBD49-069E-4149-9B0E-EC628A11B54D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D710FE45-A71C-4BDA-8A81-CF0D17CE7959}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{ED9FAEDA-F60E-42FC-910F-5E369763F547}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" activeTab="1" xr2:uid="{ED9FAEDA-F60E-42FC-910F-5E369763F547}"/>
   </bookViews>
   <sheets>
     <sheet name="Bugs and errors" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="52">
   <si>
     <t>found by</t>
   </si>
@@ -189,6 +189,9 @@
   </si>
   <si>
     <t>main</t>
+  </si>
+  <si>
+    <t>added new ways to sync data</t>
   </si>
 </sst>
 </file>
@@ -903,10 +906,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6043AC44-27D4-44BA-A4A5-A7B72C27DCEA}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1085,7 +1088,7 @@
         <v>45</v>
       </c>
       <c r="B10" s="2">
-        <v>44643</v>
+        <v>44663</v>
       </c>
       <c r="C10" t="s">
         <v>2</v>
@@ -1094,9 +1097,26 @@
         <v>48</v>
       </c>
       <c r="E10" s="1">
-        <v>44643</v>
+        <v>44664</v>
       </c>
       <c r="F10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>51</v>
+      </c>
+      <c r="B11" s="2">
+        <v>44664</v>
+      </c>
+      <c r="C11" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" s="1">
+        <v>44664</v>
+      </c>
+      <c r="F11" t="s">
         <v>50</v>
       </c>
     </row>

</xml_diff>

<commit_message>
save output data to Results folder
</commit_message>
<xml_diff>
--- a/Known python issues.xlsx
+++ b/Known python issues.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MSc\Thesis\Breaking the Higher Load\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D710FE45-A71C-4BDA-8A81-CF0D17CE7959}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5362DC00-19DD-45C7-894D-0B434AF46E44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" activeTab="1" xr2:uid="{ED9FAEDA-F60E-42FC-910F-5E369763F547}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="54">
   <si>
     <t>found by</t>
   </si>
@@ -192,6 +192,12 @@
   </si>
   <si>
     <t>added new ways to sync data</t>
+  </si>
+  <si>
+    <t>Fatigue moment logger</t>
+  </si>
+  <si>
+    <t>Added new way to log data during main</t>
   </si>
 </sst>
 </file>
@@ -906,10 +912,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6043AC44-27D4-44BA-A4A5-A7B72C27DCEA}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1120,6 +1126,26 @@
         <v>50</v>
       </c>
     </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" s="2">
+        <v>44665</v>
+      </c>
+      <c r="C12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" t="s">
+        <v>53</v>
+      </c>
+      <c r="E12" s="1">
+        <v>44665</v>
+      </c>
+      <c r="F12" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>